<commit_message>
Mise à jour 16.01.2025
</commit_message>
<xml_diff>
--- a/data/Interpol_rendement_solaire.xlsx
+++ b/data/Interpol_rendement_solaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\TM_SynergyFlex_Nikola\SynergyFlex\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AC28EF-4223-4FE1-9ABA-BC17148E8059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5032B9D-335A-4932-BA29-5C72C639EF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41440" yWindow="3040" windowWidth="28800" windowHeight="15370" xr2:uid="{A43AC8FE-A953-4253-BCE3-21B86C954AA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A43AC8FE-A953-4253-BCE3-21B86C954AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -78,15 +78,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -94,12 +100,273 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,7 +419,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CH"/>
-              <a:t>ORIENTAITON 0°</a:t>
+              <a:t>ORIENTATION 0°</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -234,10 +501,44 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.8193404085358899E-2"/>
-                  <c:y val="2.4311403951084672E-2"/>
+                  <c:x val="-0.13789195480999658"/>
+                  <c:y val="9.079511811502039E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>y = -1E-04x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t> + 0,0062x + 0,901</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2000"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1319,7 +1620,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CH"/>
-              <a:t>INVLINAISON 30 °</a:t>
+              <a:t>INCLINAISON 30 °</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1364,9 +1665,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1401,6 +1700,78 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.0436351706036745E-2"/>
+                  <c:y val="0.12755212890055409"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>y = -1E-14x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="30000"/>
+                      <a:t>6</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t> + 8E-22x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="30000"/>
+                      <a:t>5</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t> + 1E-09x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="30000"/>
+                      <a:t>4</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t> - 1E-17x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="30000"/>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t> - 4E-05x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t> - 2E-12x + 0,993</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2000"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -8849,15 +9220,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>623957</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>168966</xdr:rowOff>
+      <xdr:colOff>55218</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>27609</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>623957</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>178905</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>204304</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>129209</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9389,230 +9760,232 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B2">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="7">
         <v>-180</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>-135</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>-90</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>-45</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>45</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>90</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>135</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="8">
         <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="14">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>0.9</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>0.9</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.9</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.9</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.9</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>0.9</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>0.9</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="10">
         <v>0.9</v>
       </c>
       <c r="L3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="15">
         <v>30</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="9">
         <v>0.628</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.65600000000000003</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.77800000000000002</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.92</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>0.92</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>0.77800000000000002</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>0.65600000000000003</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="10">
         <v>0.628</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="15">
         <v>45</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <v>0.49</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.54</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.7</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.873</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <f xml:space="preserve"> (-0.00009)*A5^2 + 0.0057*A5 + 0.9025</f>
         <v>0.97675000000000001</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.873</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>0.7</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>0.54</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="10">
         <v>0.49</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="15">
         <v>60</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <v>0.377</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.47360000000000002</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.64</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.8</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>0.91</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.8</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>0.64</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>0.47360000000000002</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="10">
         <v>0.377</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="16">
         <v>90</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="11">
         <v>0.27</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <v>0.34699999999999998</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="12">
         <v>0.51</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="12">
         <v>0.6</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="12">
         <v>0.65</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="12">
         <v>0.6</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="12">
         <v>0.51</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="12">
         <v>0.34699999999999998</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="13">
         <v>0.27</v>
       </c>
     </row>

</xml_diff>